<commit_message>
another small bug fix
</commit_message>
<xml_diff>
--- a/team_data/test.xlsx
+++ b/team_data/test.xlsx
@@ -442,7 +442,7 @@
           <t>Anatomy and Physiology</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="G2" s="0" t="inlineStr">
         <is>
           <t>susan, james</t>
         </is>
@@ -477,7 +477,7 @@
           <t>Disease Detectives</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="G3" s="0" t="inlineStr">
         <is>
           <t>jennifer, james</t>
         </is>
@@ -512,12 +512,12 @@
           <t>Ecology</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="G4" s="0" t="inlineStr">
         <is>
           <t>linda, mary</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="H4" s="0" t="inlineStr">
         <is>
           <t>sarah, christopher</t>
         </is>
@@ -552,7 +552,7 @@
           <t>Entomology</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="G5" s="0" t="inlineStr">
         <is>
           <t>michael, mary</t>
         </is>
@@ -587,12 +587,12 @@
           <t>Astronomy</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="G6" s="0" t="inlineStr">
         <is>
           <t>patricia, michael</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="H6" s="0" t="inlineStr">
         <is>
           <t>karen</t>
         </is>
@@ -627,12 +627,12 @@
           <t>Optics</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="G7" s="0" t="inlineStr">
         <is>
           <t>michael, joseph</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="H7" s="0" t="inlineStr">
         <is>
           <t>robert, thomas</t>
         </is>
@@ -667,12 +667,12 @@
           <t>Fossils</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="G8" s="0" t="inlineStr">
         <is>
           <t>linda, john</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="H8" s="0" t="inlineStr">
         <is>
           <t>david, charles</t>
         </is>
@@ -767,7 +767,7 @@
           <t>Forensics</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="G11" s="0" t="inlineStr">
         <is>
           <t>jessica, joseph</t>
         </is>
@@ -832,12 +832,12 @@
           <t>Chem Lab</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="G13" s="0" t="inlineStr">
         <is>
           <t>jessica, joseph</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr">
+      <c r="H13" s="0" t="inlineStr">
         <is>
           <t>thomas</t>
         </is>
@@ -872,7 +872,7 @@
           <t>Wind Power</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr">
+      <c r="H14" s="0" t="inlineStr">
         <is>
           <t>christopher</t>
         </is>
@@ -937,12 +937,12 @@
           <t>Helicopter</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
+      <c r="G16" s="0" t="inlineStr">
         <is>
           <t>patricia, john</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr">
+      <c r="H16" s="0" t="inlineStr">
         <is>
           <t>elizabeth</t>
         </is>
@@ -977,12 +977,12 @@
           <t>Robot Tour</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
+      <c r="G17" s="0" t="inlineStr">
         <is>
           <t>mary, jennifer</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr">
+      <c r="H17" s="0" t="inlineStr">
         <is>
           <t>karen, richard</t>
         </is>
@@ -1017,9 +1017,14 @@
           <t>Tower</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
+      <c r="G18" s="0" t="inlineStr">
         <is>
           <t>barbara</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>elizabeth</t>
         </is>
       </c>
       <c r="J18" s="3" t="n">
@@ -1047,7 +1052,7 @@
           <t>Bungee Drop</t>
         </is>
       </c>
-      <c r="H19" t="inlineStr">
+      <c r="H19" s="0" t="inlineStr">
         <is>
           <t>sarah</t>
         </is>
@@ -1082,12 +1087,12 @@
           <t>Codebusters</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr">
+      <c r="G20" s="0" t="inlineStr">
         <is>
           <t>patricia, lisa</t>
         </is>
       </c>
-      <c r="H20" t="inlineStr">
+      <c r="H20" s="0" t="inlineStr">
         <is>
           <t>charles</t>
         </is>
@@ -1122,9 +1127,9 @@
           <t>Experimental Design</t>
         </is>
       </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>elizabeth, elizabeth, david</t>
+      <c r="H21" s="0" t="inlineStr">
+        <is>
+          <t>elizabeth, david</t>
         </is>
       </c>
       <c r="J21" s="3" t="n">
@@ -1157,7 +1162,7 @@
           <t>Write It Do It</t>
         </is>
       </c>
-      <c r="G22" t="inlineStr">
+      <c r="G22" s="0" t="inlineStr">
         <is>
           <t>william, susan</t>
         </is>
@@ -1192,12 +1197,12 @@
           <t>Microbe Mission</t>
         </is>
       </c>
-      <c r="G23" t="inlineStr">
+      <c r="G23" s="0" t="inlineStr">
         <is>
           <t>barbara, william</t>
         </is>
       </c>
-      <c r="H23" t="inlineStr">
+      <c r="H23" s="0" t="inlineStr">
         <is>
           <t>richard, karen</t>
         </is>

</xml_diff>

<commit_message>
added some extra checks
</commit_message>
<xml_diff>
--- a/team_data/test.xlsx
+++ b/team_data/test.xlsx
@@ -519,7 +519,7 @@
       </c>
       <c r="H4" s="0" t="inlineStr">
         <is>
-          <t>sarah, christopher</t>
+          <t>sarah</t>
         </is>
       </c>
       <c r="J4" s="3" t="n">
@@ -674,7 +674,7 @@
       </c>
       <c r="H8" s="0" t="inlineStr">
         <is>
-          <t>david, charles</t>
+          <t>charles</t>
         </is>
       </c>
       <c r="J8" s="3" t="n">
@@ -707,6 +707,11 @@
           <t>Geologic Mapping</t>
         </is>
       </c>
+      <c r="G9" s="0" t="inlineStr">
+        <is>
+          <t>christopher, elizabeth</t>
+        </is>
+      </c>
       <c r="J9" s="3" t="n">
         <v>2</v>
       </c>
@@ -737,6 +742,11 @@
           <t>Air Trajectory</t>
         </is>
       </c>
+      <c r="G10" s="0" t="inlineStr">
+        <is>
+          <t>david</t>
+        </is>
+      </c>
       <c r="J10" s="3" t="n">
         <v>2</v>
       </c>
@@ -872,11 +882,12 @@
           <t>Wind Power</t>
         </is>
       </c>
-      <c r="H14" s="0" t="inlineStr">
+      <c r="G14" s="0" t="inlineStr">
         <is>
           <t>christopher</t>
         </is>
       </c>
+      <c r="H14" s="0" t="n"/>
       <c r="J14" s="3" t="n">
         <v>2</v>
       </c>
@@ -942,11 +953,7 @@
           <t>patricia, john</t>
         </is>
       </c>
-      <c r="H16" s="0" t="inlineStr">
-        <is>
-          <t>elizabeth</t>
-        </is>
-      </c>
+      <c r="H16" s="0" t="n"/>
       <c r="J16" s="3" t="n">
         <v>2</v>
       </c>
@@ -1019,14 +1026,10 @@
       </c>
       <c r="G18" s="0" t="inlineStr">
         <is>
-          <t>barbara</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>elizabeth</t>
-        </is>
-      </c>
+          <t>barbara, elizabeth</t>
+        </is>
+      </c>
+      <c r="H18" s="0" t="n"/>
       <c r="J18" s="3" t="n">
         <v>3</v>
       </c>
@@ -1052,6 +1055,7 @@
           <t>Bungee Drop</t>
         </is>
       </c>
+      <c r="G19" s="0" t="n"/>
       <c r="H19" s="0" t="inlineStr">
         <is>
           <t>sarah</t>
@@ -1089,12 +1093,12 @@
       </c>
       <c r="G20" s="0" t="inlineStr">
         <is>
-          <t>patricia, lisa</t>
+          <t>patricia</t>
         </is>
       </c>
       <c r="H20" s="0" t="inlineStr">
         <is>
-          <t>charles</t>
+          <t>charles, lisa</t>
         </is>
       </c>
       <c r="J20" s="3" t="n">
@@ -1127,11 +1131,12 @@
           <t>Experimental Design</t>
         </is>
       </c>
-      <c r="H21" s="0" t="inlineStr">
+      <c r="G21" s="0" t="inlineStr">
         <is>
           <t>elizabeth, david</t>
         </is>
       </c>
+      <c r="H21" s="0" t="n"/>
       <c r="J21" s="3" t="n">
         <v>3</v>
       </c>

</xml_diff>